<commit_message>
These udpates correct issues with petroleum plants, removing them from being flagged as peakers, but otherwise treating them as peakers, by guaranteeing their dispatch at ~10%. This is to correct for model structure that would otherwise cause many of these plants to be built in lieu of natural gas peakers even though they are much less cost effective.
</commit_message>
<xml_diff>
--- a/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\elec\BDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\India\Models\eps-india\InputData\elec\BDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EDAECE-D7EE-4ED3-BF92-CBAE9E838988}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BDPbES!$A$1:$AK$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -124,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -367,23 +366,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -419,23 +401,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -611,10 +576,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -698,14 +663,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,147 +2129,147 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>